<commit_message>
Generation & Import Working
</commit_message>
<xml_diff>
--- a/student_information.xlsx
+++ b/student_information.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,58 +498,178 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Erica Washington</t>
+          <t>Janet Scott</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>stefanie07@example.com</t>
+          <t>deanna94@example.org</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>708.321.3242x009</t>
+          <t>557.987.3077x47839</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>001-917-395-8973x742</t>
+          <t>6462397282</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>North Lisaland</t>
+          <t>Henrymouth</t>
         </is>
       </c>
       <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2013-04-17</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1599 Amanda Plaza Suite 627, East Victoria, PW 17023</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2024-02-02</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>South Dakota</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Lynn Flores</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>charles46@example.org</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>+1-334-410-1697x5063</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>+1-813-622-9373</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Jordanville</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
         <v>12</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2008-05-25</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>49764 Bryant Square Apt. 902, Porterchester, WV 42140</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2024-02-04</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Delaware</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2006-07-02</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>62931 Chelsea Shore Suite 104, East George, IL 63484</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2024-01-31</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Frank Castro</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hernandezcrystal@example.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(339)858-7240x786</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>810-714-0034</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>West Jeffrey</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>7</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2014-03-23</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>93634 James Lane, Hansenchester, MS 17361</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2024-02-01</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Wyoming</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>None</t>
         </is>

</xml_diff>

<commit_message>
payment records fix & student queries
</commit_message>
<xml_diff>
--- a/student_information.xlsx
+++ b/student_information.xlsx
@@ -498,31 +498,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Angela Matthews</t>
+          <t>Lisa White</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>clinejessica@example.org</t>
+          <t>rachelcopeland@example.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(973)955-8656x8753</t>
+          <t>+1-850-985-4880x5059</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+1-837-393-7816</t>
+          <t>580.766.6504x18211</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jennifertown</t>
+          <t>Sancheztown</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -531,22 +531,22 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2010-03-31</t>
+          <t>2013-11-05</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>16326 Owens Fall, North Ericfort, NY 88512</t>
+          <t>9651 Julie Glens, New Erin, WI 21351</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2024-01-06</t>
+          <t>2024-01-24</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Idaho</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -558,55 +558,55 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Robert Smith</t>
+          <t>Bryan Larson</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>hannah83@example.net</t>
+          <t>waltermichael@example.org</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>256-824-5389x6225</t>
+          <t>001-725-321-2467x0153</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>9767949579</t>
+          <t>(727)597-4050x23173</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>North Eric</t>
+          <t>Port William</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2011-03-26</t>
+          <t>2007-07-17</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>735 Monique Summit Apt. 111, Danaborough, WA 36378</t>
+          <t>1043 Wise Trail, Hortonburgh, FM 55732</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2024-05-12</t>
+          <t>2024-01-09</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -618,31 +618,31 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Elizabeth Craig</t>
+          <t>Edward Cook</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pamelaboone@example.org</t>
+          <t>matthew77@example.org</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(403)442-2458x026</t>
+          <t>001-880-510-6930</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>323-570-8212x87340</t>
+          <t>339.479.2643x938</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Harriston</t>
+          <t>Hillview</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -651,22 +651,22 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2012-05-25</t>
+          <t>2012-04-22</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>375 Timothy Fields Suite 396, East Eric, TX 28157</t>
+          <t>Unit 2912 Box 9879, DPO AE 32503</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2024-05-05</t>
+          <t>2024-03-29</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">

</xml_diff>